<commit_message>
added code to dynamically enable/disable test scripts using IAnnotationTransformer and some restructuring of packages
</commit_message>
<xml_diff>
--- a/src/main/java/com/trainline/qa/testData/TestDocument.xlsx
+++ b/src/main/java/com/trainline/qa/testData/TestDocument.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{3D5F5779-C7DE-4A4A-84D3-B0385D642084}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1003BB0E-55CB-40B7-BAD9-43E7F6BE597A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10068" windowHeight="7584" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="4" r:id="rId2"/>
     <sheet name="Cookie" sheetId="3" r:id="rId3"/>
+    <sheet name="TestScripts" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
   <si>
     <t>Deepak</t>
   </si>
@@ -125,6 +125,15 @@
   </si>
   <si>
     <t>Gajanana Society</t>
+  </si>
+  <si>
+    <t>TestName</t>
+  </si>
+  <si>
+    <t>Enabled</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AnnotationTtest </t>
   </si>
 </sst>
 </file>
@@ -573,7 +582,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{107D4962-AC65-438D-8689-9A16F1ED8D86}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -736,4 +745,38 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FEEB11A-B40C-46D4-A57F-2FFDDA4EBE53}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="32" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
changed retry code. Made transform method synchronised for parallel execution.
</commit_message>
<xml_diff>
--- a/src/main/java/com/trainline/qa/testData/TestDocument.xlsx
+++ b/src/main/java/com/trainline/qa/testData/TestDocument.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1003BB0E-55CB-40B7-BAD9-43E7F6BE597A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5891616F-4AA5-4FD5-ABD8-FC59FE034805}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -133,7 +133,7 @@
     <t>Enabled</t>
   </si>
   <si>
-    <t xml:space="preserve">AnnotationTtest </t>
+    <t xml:space="preserve">annotationTest </t>
   </si>
 </sst>
 </file>
@@ -752,12 +752,13 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32" customWidth="1"/>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>